<commit_message>
Fix for the annotator selenium-test
</commit_message>
<xml_diff>
--- a/src/test/resources/test_file.xlsx
+++ b/src/test/resources/test_file.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="1260" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7060" yWindow="1260" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="2" r:id="rId1"/>
@@ -313,21 +313,6 @@
     <t>FATHMMScore</t>
   </si>
   <si>
-    <t>1000Gp1_FreqAll</t>
-  </si>
-  <si>
-    <t>1000Gp1_FreqAFR</t>
-  </si>
-  <si>
-    <t>1000Gp1_FreqEUR</t>
-  </si>
-  <si>
-    <t>1000Gp1_FreqAMR</t>
-  </si>
-  <si>
-    <t>1000Gp1_FreqASN</t>
-  </si>
-  <si>
     <t>hgmdAccession</t>
   </si>
   <si>
@@ -737,6 +722,21 @@
   </si>
   <si>
     <t>test_entity</t>
+  </si>
+  <si>
+    <t>D1000Gp1_FreqAll</t>
+  </si>
+  <si>
+    <t>D1000Gp1_FreqAFR</t>
+  </si>
+  <si>
+    <t>D1000Gp1_FreqEUR</t>
+  </si>
+  <si>
+    <t>D1000Gp1_FreqAMR</t>
+  </si>
+  <si>
+    <t>D1000Gp1_FreqASN</t>
   </si>
 </sst>
 </file>
@@ -1184,13 +1184,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1249,7 +1249,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1266,7 +1266,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1274,10 +1274,10 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1285,10 +1285,10 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1296,7 +1296,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1304,10 +1304,10 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1315,7 +1315,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1323,7 +1323,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1331,10 +1331,10 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1342,10 +1342,10 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1353,10 +1353,10 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1364,10 +1364,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1375,10 +1375,10 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1386,32 +1386,32 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1419,10 +1419,10 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1430,10 +1430,10 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1441,10 +1441,10 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1452,10 +1452,10 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1463,10 +1463,10 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1474,10 +1474,10 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1485,10 +1485,10 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1496,10 +1496,10 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1507,10 +1507,10 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1518,10 +1518,10 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1529,21 +1529,21 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1551,10 +1551,10 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1562,10 +1562,10 @@
         <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1573,10 +1573,10 @@
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1584,10 +1584,10 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1595,10 +1595,10 @@
         <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1606,10 +1606,10 @@
         <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1617,10 +1617,10 @@
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1628,10 +1628,10 @@
         <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1639,10 +1639,10 @@
         <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1650,10 +1650,10 @@
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1661,10 +1661,10 @@
         <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1672,10 +1672,10 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1683,10 +1683,10 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1694,10 +1694,10 @@
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1705,10 +1705,10 @@
         <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1716,10 +1716,10 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1727,10 +1727,10 @@
         <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1738,10 +1738,10 @@
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1749,10 +1749,10 @@
         <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1760,10 +1760,10 @@
         <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1771,10 +1771,10 @@
         <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1782,10 +1782,10 @@
         <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1793,10 +1793,10 @@
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1804,10 +1804,10 @@
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1815,10 +1815,10 @@
         <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1826,10 +1826,10 @@
         <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1837,10 +1837,10 @@
         <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1848,10 +1848,10 @@
         <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1859,10 +1859,10 @@
         <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1870,10 +1870,10 @@
         <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1881,10 +1881,10 @@
         <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1892,10 +1892,10 @@
         <v>72</v>
       </c>
       <c r="B61" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C61" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1903,10 +1903,10 @@
         <v>73</v>
       </c>
       <c r="B62" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C62" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1914,10 +1914,10 @@
         <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1925,10 +1925,10 @@
         <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C64" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1936,10 +1936,10 @@
         <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C65" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1947,10 +1947,10 @@
         <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C66" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1958,10 +1958,10 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1969,10 +1969,10 @@
         <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1980,10 +1980,10 @@
         <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C69" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1991,10 +1991,10 @@
         <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C70" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2002,10 +2002,10 @@
         <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C71" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2013,10 +2013,10 @@
         <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C72" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2024,10 +2024,10 @@
         <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2035,10 +2035,10 @@
         <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C74" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2046,10 +2046,10 @@
         <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C75" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2057,10 +2057,10 @@
         <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C76" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2068,10 +2068,10 @@
         <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2079,10 +2079,10 @@
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C78" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2090,10 +2090,10 @@
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2101,10 +2101,10 @@
         <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C80" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2112,10 +2112,10 @@
         <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C81" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2123,10 +2123,10 @@
         <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C82" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2134,10 +2134,10 @@
         <v>94</v>
       </c>
       <c r="B83" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2145,10 +2145,10 @@
         <v>95</v>
       </c>
       <c r="B84" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2156,153 +2156,153 @@
         <v>96</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C85" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>234</v>
       </c>
       <c r="B86" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C86" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>235</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>99</v>
+        <v>236</v>
       </c>
       <c r="B88" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>237</v>
       </c>
       <c r="B89" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C89" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="B90" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C92" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C93" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C94" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C95" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C96" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C97" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C98" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2320,11 +2320,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="CL3" sqref="CL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="83" max="83" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:97">
       <c r="A1" t="s">
@@ -2370,10 +2380,10 @@
         <v>29</v>
       </c>
       <c r="O1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="P1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q1" t="s">
         <v>30</v>
@@ -2409,7 +2419,7 @@
         <v>40</v>
       </c>
       <c r="AB1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="AC1" t="s">
         <v>41</v>
@@ -2580,43 +2590,43 @@
         <v>96</v>
       </c>
       <c r="CG1" t="s">
+        <v>234</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>235</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>236</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>237</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>238</v>
+      </c>
+      <c r="CL1" t="s">
         <v>97</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CM1" t="s">
         <v>98</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CN1" t="s">
         <v>99</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CO1" t="s">
         <v>100</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CP1" t="s">
         <v>101</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CQ1" t="s">
         <v>102</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CR1" t="s">
         <v>103</v>
       </c>
-      <c r="CN1" t="s">
-        <v>104</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>105</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>106</v>
-      </c>
-      <c r="CQ1" t="s">
+      <c r="CS1" t="s">
         <v>107</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:97">
@@ -2633,19 +2643,19 @@
         <v>6511791</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N2">
         <v>606351</v>
@@ -2660,49 +2670,49 @@
         <v>59</v>
       </c>
       <c r="Y2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF2" t="s">
         <v>120</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>125</v>
       </c>
       <c r="AG2">
         <v>9</v>
       </c>
       <c r="AH2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN2" t="s">
         <v>126</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>131</v>
       </c>
       <c r="AO2">
         <v>3531</v>
@@ -2711,10 +2721,10 @@
         <v>-18</v>
       </c>
       <c r="AR2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AS2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="AT2">
         <v>-2</v>
@@ -2729,34 +2739,34 @@
         <v>-22178</v>
       </c>
       <c r="BP2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BU2" t="s">
         <v>134</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BV2" t="s">
         <v>135</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BW2" t="s">
         <v>136</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BZ2" t="s">
         <v>137</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="CA2" t="s">
         <v>138</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>139</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>141</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>142</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>143</v>
       </c>
       <c r="CB2" s="3">
         <v>1241</v>
@@ -2768,10 +2778,10 @@
         <v>1935</v>
       </c>
       <c r="CE2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="CF2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:97">
@@ -2788,22 +2798,22 @@
         <v>9324282</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="M3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="N3">
         <v>138090</v>
@@ -2818,49 +2828,49 @@
         <v>98</v>
       </c>
       <c r="Y3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF3" t="s">
         <v>120</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>125</v>
       </c>
       <c r="AG3">
         <v>5</v>
       </c>
       <c r="AH3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="AI3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="AJ3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AK3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="AL3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="AM3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="AN3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AO3">
         <v>9115</v>
@@ -2869,10 +2879,10 @@
         <v>715</v>
       </c>
       <c r="AR3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="AS3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="AT3">
         <v>1</v>
@@ -2884,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="AW3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AY3">
         <v>137</v>
@@ -2893,13 +2903,13 @@
         <v>137</v>
       </c>
       <c r="BA3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="BB3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="BE3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="BF3">
         <v>0</v>
@@ -2908,79 +2918,79 @@
         <v>43</v>
       </c>
       <c r="BH3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="BI3" t="s">
+        <v>154</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>156</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>158</v>
+      </c>
+      <c r="BN3" t="s">
         <v>159</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>160</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>161</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>163</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>164</v>
       </c>
       <c r="BO3" s="3">
         <v>-15533</v>
       </c>
       <c r="BP3" t="s">
+        <v>160</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>161</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>162</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>163</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>164</v>
+      </c>
+      <c r="BX3" t="s">
         <v>165</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="BY3" t="s">
         <v>166</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="BZ3" t="s">
         <v>167</v>
       </c>
-      <c r="BS3" t="s">
-        <v>138</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>138</v>
-      </c>
-      <c r="BU3" t="s">
+      <c r="CA3" t="s">
         <v>168</v>
       </c>
-      <c r="BV3" t="s">
-        <v>140</v>
-      </c>
-      <c r="BW3" t="s">
+      <c r="CB3" t="s">
         <v>169</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>170</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>171</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>172</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>173</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>174</v>
       </c>
       <c r="CC3" s="3">
         <v>11147</v>
       </c>
       <c r="CD3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="CE3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="CF3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:97">
@@ -2997,22 +3007,22 @@
         <v>22156531</v>
       </c>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="M4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="N4">
         <v>142461</v>
@@ -3027,49 +3037,49 @@
         <v>44</v>
       </c>
       <c r="Y4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF4" t="s">
         <v>120</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>125</v>
       </c>
       <c r="AG4">
         <v>86</v>
       </c>
       <c r="AH4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN4" t="s">
         <v>182</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>183</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>183</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>187</v>
       </c>
       <c r="AO4">
         <v>14288</v>
@@ -3078,10 +3088,10 @@
         <v>-46</v>
       </c>
       <c r="AR4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="AS4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="AT4">
         <v>-1</v>
@@ -3093,7 +3103,7 @@
         <v>-2</v>
       </c>
       <c r="AW4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AY4">
         <v>137</v>
@@ -3102,49 +3112,49 @@
         <v>137</v>
       </c>
       <c r="BA4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="BB4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="BP4" t="s">
+        <v>185</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>186</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>187</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>188</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>189</v>
+      </c>
+      <c r="BX4" t="s">
         <v>190</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BY4" t="s">
+        <v>166</v>
+      </c>
+      <c r="BZ4" t="s">
         <v>191</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="CA4" t="s">
         <v>192</v>
       </c>
-      <c r="BS4" t="s">
-        <v>137</v>
-      </c>
-      <c r="BT4" t="s">
-        <v>138</v>
-      </c>
-      <c r="BU4" t="s">
+      <c r="CB4" t="s">
         <v>193</v>
-      </c>
-      <c r="BV4" t="s">
-        <v>140</v>
-      </c>
-      <c r="BW4" t="s">
-        <v>194</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>195</v>
-      </c>
-      <c r="BY4" t="s">
-        <v>171</v>
-      </c>
-      <c r="BZ4" t="s">
-        <v>196</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>197</v>
-      </c>
-      <c r="CB4" t="s">
-        <v>198</v>
       </c>
       <c r="CC4" s="3">
         <v>6978</v>
@@ -3153,10 +3163,10 @@
         <v>2285</v>
       </c>
       <c r="CE4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="CF4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:97">
@@ -3173,22 +3183,22 @@
         <v>94487490</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="M5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="N5">
         <v>601691</v>
@@ -3206,49 +3216,49 @@
         <v>51</v>
       </c>
       <c r="Y5" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF5" t="s">
         <v>120</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>202</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>203</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>200</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>125</v>
       </c>
       <c r="AG5">
         <v>33</v>
       </c>
       <c r="AH5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="AI5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AJ5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="AK5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AL5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AM5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AN5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AO5">
         <v>7325</v>
@@ -3257,10 +3267,10 @@
         <v>18</v>
       </c>
       <c r="AR5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="AS5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="AT5">
         <v>-1</v>
@@ -3272,7 +3282,7 @@
         <v>-1</v>
       </c>
       <c r="AW5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AY5">
         <v>89</v>
@@ -3281,79 +3291,79 @@
         <v>137</v>
       </c>
       <c r="BA5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="BB5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="BD5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="BE5">
         <v>5</v>
       </c>
       <c r="BF5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="BG5">
         <v>89</v>
       </c>
       <c r="BH5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="BI5" t="s">
+        <v>209</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>210</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>211</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>212</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN5" t="s">
         <v>214</v>
       </c>
-      <c r="BJ5" t="s">
+      <c r="BP5" t="s">
+        <v>161</v>
+      </c>
+      <c r="BQ5" t="s">
         <v>215</v>
       </c>
-      <c r="BK5" t="s">
+      <c r="BR5" t="s">
         <v>216</v>
       </c>
-      <c r="BL5" t="s">
+      <c r="BS5" t="s">
+        <v>133</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>133</v>
+      </c>
+      <c r="BU5" t="s">
         <v>217</v>
       </c>
-      <c r="BM5" t="s">
+      <c r="BV5" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW5" t="s">
         <v>218</v>
       </c>
-      <c r="BN5" t="s">
+      <c r="BX5" t="s">
         <v>219</v>
       </c>
-      <c r="BP5" t="s">
+      <c r="BY5" t="s">
         <v>166</v>
       </c>
-      <c r="BQ5" t="s">
+      <c r="BZ5" t="s">
         <v>220</v>
       </c>
-      <c r="BR5" t="s">
+      <c r="CA5" t="s">
         <v>221</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>138</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>138</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>222</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>140</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>223</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>224</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>171</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>225</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>226</v>
       </c>
       <c r="CB5" s="3">
         <v>2326</v>
@@ -3362,40 +3372,40 @@
         <v>11685</v>
       </c>
       <c r="CD5" t="s">
+        <v>222</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>223</v>
+      </c>
+      <c r="CF5" t="s">
+        <v>224</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>225</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>226</v>
+      </c>
+      <c r="CL5" t="s">
         <v>227</v>
-      </c>
-      <c r="CE5" t="s">
-        <v>228</v>
-      </c>
-      <c r="CF5" t="s">
-        <v>229</v>
-      </c>
-      <c r="CG5" t="s">
-        <v>230</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>231</v>
-      </c>
-      <c r="CL5" t="s">
-        <v>232</v>
       </c>
       <c r="CM5">
         <v>9295268.2314346004</v>
       </c>
       <c r="CN5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CO5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="CP5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="CQ5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="CR5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>